<commit_message>
ropecon scenario starts to form
</commit_message>
<xml_diff>
--- a/ep-corporations.xlsx
+++ b/ep-corporations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dare/Documents/personal/rpg/posthuman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B87B83-6487-B042-BC1E-D249E5D09B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821F3AA6-2848-9F43-A170-5765278606B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{5839D7C6-F340-2849-BC89-4905B8F141B1}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="849">
   <si>
     <t>Cythera (Venus)</t>
   </si>
@@ -2574,6 +2574,18 @@
   </si>
   <si>
     <t>Noctis-Quanjiao (Mars). Low-end synths &amp;  casemorphs</t>
+  </si>
+  <si>
+    <t>Biotech</t>
+  </si>
+  <si>
+    <t>Senray</t>
+  </si>
+  <si>
+    <t>HORIZ</t>
+  </si>
+  <si>
+    <t>Locus</t>
   </si>
 </sst>
 </file>
@@ -2967,11 +2979,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AB6C51-22ED-3F49-B833-91C693E9FCD1}">
-  <dimension ref="A1:I264"/>
+  <dimension ref="A1:I265"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I163" sqref="I163"/>
+      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A265" sqref="A265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8480,11 +8492,31 @@
         <v>499</v>
       </c>
     </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>846</v>
+      </c>
+      <c r="D265" t="s">
+        <v>847</v>
+      </c>
+      <c r="E265" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="F265" t="s">
+        <v>701</v>
+      </c>
+      <c r="G265" t="s">
+        <v>848</v>
+      </c>
+      <c r="H265" t="s">
+        <v>845</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I264">
     <sortCondition ref="A2:A264"/>
   </sortState>
-  <conditionalFormatting sqref="A2:N75 A76:E77 G76:N77 A78:N120 F121 A121:E122 G121:N122 A123:N254 F255:H255 A255:A259 D255:D264 F256:F258 H256:I259 F260:I264 A261 A263:A264">
+  <conditionalFormatting sqref="A2:N75 A76:E77 G76:N77 A78:N120 F121 A121:E122 G121:N122 A123:N254 F255:H255 A255:A259 F256:F258 H256:I259 F260:I264 A261 A263:A265 D255:D265 F265:H265">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>$B2&gt;0</formula>
     </cfRule>

</xml_diff>